<commit_message>
Prod Def + Arch Take II
updates to:
- Funtionality List
- Camera Flow Diagram
- Behavior Definition
- Block Diagram
- Prod Arch
- Major Component BOM
</commit_message>
<xml_diff>
--- a/Jamica/EWC Architecture/EWC Major Component BOM.xlsx
+++ b/Jamica/EWC Architecture/EWC Major Component BOM.xlsx
@@ -9,10 +9,10 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1340" yWindow="2000" windowWidth="23200" windowHeight="11620"/>
+    <workbookView xWindow="33420" yWindow="2880" windowWidth="23200" windowHeight="11620"/>
   </bookViews>
   <sheets>
-    <sheet name="ArduinoElectronicLoad_FullBOM" sheetId="1" r:id="rId1"/>
+    <sheet name="Embeddded Wearable Camera BOM" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
   <si>
     <t>Qty</t>
   </si>
@@ -32,15 +32,6 @@
     <t>Value</t>
   </si>
   <si>
-    <t>Device</t>
-  </si>
-  <si>
-    <t>Package</t>
-  </si>
-  <si>
-    <t>Parts</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -50,31 +41,10 @@
     <t>MANUFACTURER</t>
   </si>
   <si>
-    <t>MFG_PART_NUMBER</t>
-  </si>
-  <si>
-    <t>PACKAGE</t>
-  </si>
-  <si>
     <t>VENDOR</t>
   </si>
   <si>
     <t>VENDOR_PART_NUM</t>
-  </si>
-  <si>
-    <t>CAP CER 0.1UF 16V X7R 0603</t>
-  </si>
-  <si>
-    <t>RES SMD 1.1K OHM 1% 1/10W 0603</t>
-  </si>
-  <si>
-    <t>RES SMD 100K OHM 1% 1/10W 0603</t>
-  </si>
-  <si>
-    <t>THERMISTOR 10K OHM NTC 0402 SMD</t>
-  </si>
-  <si>
-    <t>RES SMD 10K OHM 1% 1/10W 0603</t>
   </si>
   <si>
     <r>
@@ -164,29 +134,33 @@
     <t>Shenzhen PkCell Battery Co., LTD</t>
   </si>
   <si>
-    <t>LP503035</t>
-  </si>
-  <si>
-    <t>PN001</t>
-  </si>
-  <si>
-    <t>PN002</t>
-  </si>
-  <si>
-    <t>PN003</t>
-  </si>
-  <si>
-    <t>PN004</t>
-  </si>
-  <si>
-    <t>PN005</t>
+    <t>Included above</t>
+  </si>
+  <si>
+    <t>Processor</t>
+  </si>
+  <si>
+    <t>Processor-compatible camera</t>
+  </si>
+  <si>
+    <t>Camera ribbon cable</t>
+  </si>
+  <si>
+    <t>Charger</t>
+  </si>
+  <si>
+    <t>Rechargable lithium ion battery</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0;[Red]\-&quot;$&quot;#,##0"/>
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
+  </numFmts>
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -318,6 +292,22 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -635,7 +625,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -678,14 +668,21 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="44">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -714,11 +711,13 @@
     <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
     <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -1029,57 +1028,52 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L32"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.1640625" customWidth="1"/>
     <col min="2" max="2" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5" customWidth="1"/>
-    <col min="4" max="4" width="16.33203125" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" customWidth="1"/>
-    <col min="6" max="6" width="36.83203125" customWidth="1"/>
-    <col min="7" max="7" width="44.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="32.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.83203125" customWidth="1"/>
+    <col min="4" max="4" width="44.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.33203125" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" customWidth="1"/>
+    <col min="7" max="7" width="22.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
@@ -1101,175 +1095,123 @@
       <c r="G7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>1</v>
       </c>
-      <c r="B8" s="3"/>
+      <c r="B8" s="4">
+        <v>10</v>
+      </c>
       <c r="C8" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
+        <v>12</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="F8" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3">
-        <v>603</v>
-      </c>
-      <c r="K8" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="L8" s="3">
+        <v>17</v>
+      </c>
+      <c r="G8" s="3">
         <v>3400</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>1</v>
       </c>
-      <c r="B9" s="3"/>
+      <c r="B9" s="5">
+        <v>29.95</v>
+      </c>
       <c r="C9" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
+        <v>13</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="F9" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3">
-        <v>603</v>
-      </c>
-      <c r="K9" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="L9" s="3">
+        <v>17</v>
+      </c>
+      <c r="G9" s="3">
         <v>3100</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>1</v>
       </c>
-      <c r="B10" s="3"/>
+      <c r="B10" s="6" t="s">
+        <v>20</v>
+      </c>
       <c r="C10" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
+        <v>14</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="F10" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3">
-        <v>603</v>
-      </c>
-      <c r="K10" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="L10" s="3">
+        <v>17</v>
+      </c>
+      <c r="G10" s="3">
         <v>3157</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>1</v>
       </c>
-      <c r="B11" s="3"/>
+      <c r="B11" s="5">
+        <v>9.9499999999999993</v>
+      </c>
       <c r="C11" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
+        <v>15</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>17</v>
+      </c>
       <c r="F11" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3">
-        <v>402</v>
-      </c>
-      <c r="K11" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="L11" s="3">
+        <v>17</v>
+      </c>
+      <c r="G11" s="3">
         <v>1944</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>1</v>
       </c>
-      <c r="B12" s="3"/>
+      <c r="B12" s="5">
+        <v>7.95</v>
+      </c>
       <c r="C12" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
+        <v>16</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="F12" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="I12" t="s">
-        <v>30</v>
-      </c>
-      <c r="J12" s="3">
-        <v>603</v>
-      </c>
-      <c r="K12" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="L12" s="3">
+        <v>17</v>
+      </c>
+      <c r="G12" s="3">
         <v>1578</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -1277,13 +1219,8 @@
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -1291,13 +1228,8 @@
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -1305,13 +1237,8 @@
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -1319,13 +1246,8 @@
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -1333,13 +1255,8 @@
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -1347,13 +1264,8 @@
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -1361,13 +1273,8 @@
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -1375,13 +1282,8 @@
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="L20" s="3"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -1389,13 +1291,8 @@
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="3"/>
-      <c r="L21" s="3"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -1403,13 +1300,8 @@
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
-      <c r="K22" s="3"/>
-      <c r="L22" s="3"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -1417,13 +1309,8 @@
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
-      <c r="J23" s="3"/>
-      <c r="K23" s="3"/>
-      <c r="L23" s="3"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -1431,13 +1318,8 @@
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
-      <c r="J24" s="3"/>
-      <c r="K24" s="3"/>
-      <c r="L24" s="3"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -1445,13 +1327,8 @@
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
-      <c r="K25" s="3"/>
-      <c r="L25" s="3"/>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -1459,13 +1336,8 @@
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="3"/>
-      <c r="J26" s="3"/>
-      <c r="K26" s="3"/>
-      <c r="L26" s="3"/>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -1473,13 +1345,8 @@
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
-      <c r="I27" s="3"/>
-      <c r="J27" s="3"/>
-      <c r="K27" s="3"/>
-      <c r="L27" s="3"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -1487,13 +1354,8 @@
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
-      <c r="I28" s="3"/>
-      <c r="J28" s="3"/>
-      <c r="K28" s="3"/>
-      <c r="L28" s="3"/>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -1501,13 +1363,8 @@
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
-      <c r="I29" s="3"/>
-      <c r="J29" s="3"/>
-      <c r="K29" s="3"/>
-      <c r="L29" s="3"/>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -1515,13 +1372,8 @@
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
-      <c r="I30" s="3"/>
-      <c r="J30" s="3"/>
-      <c r="K30" s="3"/>
-      <c r="L30" s="3"/>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -1529,13 +1381,8 @@
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
-      <c r="I31" s="3"/>
-      <c r="J31" s="3"/>
-      <c r="K31" s="3"/>
-      <c r="L31" s="3"/>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -1543,11 +1390,6 @@
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
-      <c r="H32" s="3"/>
-      <c r="I32" s="3"/>
-      <c r="J32" s="3"/>
-      <c r="K32" s="3"/>
-      <c r="L32" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>